<commit_message>
edited consumption table method and added political data processing
</commit_message>
<xml_diff>
--- a/consumption_tables/Total energy consumption._              Billion Btu/All petroleum products total consumption._                              Billion Btu.xlsx
+++ b/consumption_tables/Total energy consumption._              Billion Btu/All petroleum products total consumption._                              Billion Btu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
   <si>
     <t>StateCode</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>ChangeConsumptionPerCapita</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>38.78044729944203%</t>
+  </si>
+  <si>
+    <t>39.37563216759075%</t>
+  </si>
+  <si>
+    <t>0.5951848681487206%</t>
   </si>
   <si>
     <t>AL</t>
@@ -714,8 +726,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -1013,7 +1025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1067,19 +1079,19 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>483003</v>
+        <v>226510</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>546367</v>
+        <v>244086</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1.131187590967344</v>
+        <v>1.077594808176239</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4050000</v>
+        <v>553000</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>4854000</v>
+        <v>738000</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -1090,14 +1102,14 @@
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>0.11926</v>
+      <c r="K2" s="3" t="n">
+        <v>0.4096021699819168</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>0.1125601565718995</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>-0.006699843428100538</v>
+        <v>0.330739837398374</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>-0.07886233258354286</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1108,19 +1120,19 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>266051</v>
+        <v>483003</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>327611</v>
+        <v>546367</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1.231384208290892</v>
+        <v>1.131187590967344</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2357000</v>
+        <v>4050000</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>2978000</v>
+        <v>4854000</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>17</v>
@@ -1132,13 +1144,13 @@
         <v>19</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.1128769622401358</v>
+        <v>0.11926</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.1100104096709201</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>-0.002866552569215683</v>
+        <v>0.1125601565718995</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>-0.006699843428100538</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1149,19 +1161,19 @@
         <v>20</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>347299</v>
+        <v>266051</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>530755</v>
+        <v>327611</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1.528236476350349</v>
+        <v>1.231384208290892</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>3684000</v>
+        <v>2357000</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>6818000</v>
+        <v>2978000</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -1173,13 +1185,13 @@
         <v>23</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.09427225841476655</v>
+        <v>0.1128769622401358</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.07784614256380171</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>-0.01642611585096485</v>
+        <v>0.1100104096709201</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>-0.002866552569215683</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1190,19 +1202,19 @@
         <v>24</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>3506974</v>
+        <v>347299</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>3491679</v>
+        <v>530755</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.9956386902212563</v>
+        <v>1.528236476350349</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>29960000</v>
+        <v>3684000</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>38994000</v>
+        <v>6818000</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>25</v>
@@ -1214,13 +1226,13 @@
         <v>27</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.1170552069425901</v>
+        <v>0.09427225841476655</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.08954400677027236</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>-0.02751120017231777</v>
+        <v>0.07784614256380171</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>-0.01642611585096485</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1231,19 +1243,19 @@
         <v>28</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>326575</v>
+        <v>3506974</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>484154</v>
+        <v>3491679</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1.482520094924596</v>
+        <v>0.9956386902212563</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>3308000</v>
+        <v>29960000</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>5449000</v>
+        <v>38994000</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>29</v>
@@ -1255,13 +1267,13 @@
         <v>31</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.09872279322853689</v>
+        <v>0.1170552069425901</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.08885189943108827</v>
-      </c>
-      <c r="M6" s="3" t="n">
-        <v>-0.009870893797448613</v>
+        <v>0.08954400677027236</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>-0.02751120017231777</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1272,19 +1284,19 @@
         <v>32</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>439536</v>
+        <v>326575</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>327342</v>
+        <v>484154</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.7447444577918533</v>
+        <v>1.482520094924596</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>3292000</v>
+        <v>3308000</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>3585000</v>
+        <v>5449000</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>33</v>
@@ -1296,13 +1308,13 @@
         <v>35</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1335164034021871</v>
+        <v>0.09872279322853689</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.09130878661087866</v>
-      </c>
-      <c r="M7" s="3" t="n">
-        <v>-0.04220761679130847</v>
+        <v>0.08885189943108827</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>-0.009870893797448613</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1313,19 +1325,19 @@
         <v>36</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>139535</v>
+        <v>439536</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>106377</v>
+        <v>327342</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.7623678646934461</v>
+        <v>0.7447444577918533</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>670000</v>
+        <v>3292000</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>944000</v>
+        <v>3585000</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>37</v>
@@ -1337,13 +1349,13 @@
         <v>39</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.2082611940298507</v>
+        <v>0.1335164034021871</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.1126875</v>
-      </c>
-      <c r="M8" s="3" t="n">
-        <v>-0.09557369402985075</v>
+        <v>0.09130878661087866</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <v>-0.04220761679130847</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1354,19 +1366,19 @@
         <v>40</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1567567</v>
+        <v>139535</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1688401</v>
+        <v>106377</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>1.077083786530336</v>
+        <v>0.7623678646934461</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13033000</v>
+        <v>670000</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>20245000</v>
+        <v>944000</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>41</v>
@@ -1378,13 +1390,13 @@
         <v>43</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.1202767589963938</v>
+        <v>0.2082611940298507</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.08339841936280563</v>
-      </c>
-      <c r="M9" s="3" t="n">
-        <v>-0.03687833963358814</v>
+        <v>0.1126875</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <v>-0.09557369402985075</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1395,19 +1407,19 @@
         <v>44</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>815682</v>
+        <v>1567567</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>917043</v>
+        <v>1688401</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1.124265338698169</v>
+        <v>1.077083786530336</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>6513000</v>
+        <v>13033000</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>10199000</v>
+        <v>20245000</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>45</v>
@@ -1419,13 +1431,13 @@
         <v>47</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.1252390603408567</v>
+        <v>0.1202767589963938</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.0899149916658496</v>
-      </c>
-      <c r="M10" s="3" t="n">
-        <v>-0.03532406867500715</v>
+        <v>0.08339841936280563</v>
+      </c>
+      <c r="M10" s="4" t="n">
+        <v>-0.03687833963358814</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1436,37 +1448,37 @@
         <v>48</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>292763</v>
+        <v>815682</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>241701</v>
+        <v>917043</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.8255858834620495</v>
+        <v>1.124265338698169</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1113000</v>
+        <v>6513000</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>1425000</v>
-      </c>
-      <c r="H11" s="4" t="s">
+        <v>10199000</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>50</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>51</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.2630395327942498</v>
+        <v>0.1252390603408567</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.1696147368421053</v>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>-0.09342479595214453</v>
+        <v>0.0899149916658496</v>
+      </c>
+      <c r="M11" s="4" t="n">
+        <v>-0.03532406867500715</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1477,37 +1489,37 @@
         <v>52</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>304897</v>
+        <v>292763</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>433318</v>
+        <v>241701</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>1.421194698537539</v>
+        <v>0.8255858834620495</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>2781000</v>
+        <v>1113000</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>3122000</v>
-      </c>
-      <c r="H12" s="2" t="s">
+        <v>1425000</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>0.1096357425386552</v>
+        <v>0.2630395327942498</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.1387950032030749</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>0.02915926066441979</v>
+        <v>0.1696147368421053</v>
+      </c>
+      <c r="M12" s="4" t="n">
+        <v>-0.09342479595214453</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1518,19 +1530,19 @@
         <v>56</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>120137</v>
+        <v>304897</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>178336</v>
+        <v>433318</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>1.484438599265838</v>
+        <v>1.421194698537539</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1012000</v>
+        <v>2781000</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>1653000</v>
+        <v>3122000</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>57</v>
@@ -1542,13 +1554,13 @@
         <v>59</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>0.1187124505928854</v>
+        <v>0.1096357425386552</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0.1078862673926195</v>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>-0.01082618320026589</v>
+        <v>0.1387950032030749</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>0.02915926066441979</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1559,19 +1571,19 @@
         <v>60</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>1101969</v>
+        <v>120137</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>1315204</v>
+        <v>178336</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>1.193503628504976</v>
+        <v>1.484438599265838</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>11453000</v>
+        <v>1012000</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>12839000</v>
+        <v>1653000</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>61</v>
@@ -1583,13 +1595,13 @@
         <v>63</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>0.09621662446520562</v>
+        <v>0.1187124505928854</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0.1024381961211932</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>0.006221571655987621</v>
+        <v>0.1078862673926195</v>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>-0.01082618320026589</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1600,19 +1612,19 @@
         <v>64</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>816542</v>
+        <v>1101969</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>803572</v>
+        <v>1315204</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.9841159425969516</v>
+        <v>1.193503628504976</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>5558000</v>
+        <v>11453000</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>6613000</v>
+        <v>12839000</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>65</v>
@@ -1624,13 +1636,13 @@
         <v>67</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0.146912918315941</v>
+        <v>0.09621662446520562</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0.1215139876001815</v>
-      </c>
-      <c r="M15" s="3" t="n">
-        <v>-0.02539893071575954</v>
+        <v>0.1024381961211932</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0.006221571655987621</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1641,19 +1653,19 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>400748</v>
+        <v>816542</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>354990</v>
+        <v>803572</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.8858185193687804</v>
+        <v>0.9841159425969516</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>2481000</v>
+        <v>5558000</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>2907000</v>
+        <v>6613000</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>69</v>
@@ -1665,13 +1677,13 @@
         <v>71</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0.1615268037081822</v>
+        <v>0.146912918315941</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.1221155830753354</v>
-      </c>
-      <c r="M16" s="3" t="n">
-        <v>-0.03941122063284679</v>
+        <v>0.1215139876001815</v>
+      </c>
+      <c r="M16" s="4" t="n">
+        <v>-0.02539893071575954</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1682,19 +1694,19 @@
         <v>72</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>502009</v>
+        <v>400748</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>607832</v>
+        <v>354990</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>1.21079900957951</v>
+        <v>0.8858185193687804</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>3694000</v>
+        <v>2481000</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>4425000</v>
+        <v>2907000</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>73</v>
@@ -1706,13 +1718,13 @@
         <v>75</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.1358984840281538</v>
+        <v>0.1615268037081822</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0.1373631638418079</v>
-      </c>
-      <c r="M17" s="2" t="n">
-        <v>0.001464679813654141</v>
+        <v>0.1221155830753354</v>
+      </c>
+      <c r="M17" s="4" t="n">
+        <v>-0.03941122063284679</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1723,19 +1735,19 @@
         <v>76</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>1616832</v>
+        <v>502009</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2100885</v>
+        <v>607832</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1.299383609428809</v>
+        <v>1.21079900957951</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>4222000</v>
+        <v>3694000</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>4669000</v>
+        <v>4425000</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>77</v>
@@ -1743,17 +1755,17 @@
       <c r="I18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="4" t="n">
-        <v>0.3829540502131691</v>
-      </c>
-      <c r="L18" s="4" t="n">
-        <v>0.4499646605268794</v>
+      <c r="K18" s="2" t="n">
+        <v>0.1358984840281538</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0.1373631638418079</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0.06701061031371025</v>
+        <v>0.001464679813654141</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1764,19 +1776,19 @@
         <v>80</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>806247</v>
+        <v>1616832</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>585019</v>
+        <v>2100885</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.7256076611757936</v>
+        <v>1.299383609428809</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>6023000</v>
+        <v>4222000</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>6784000</v>
+        <v>4669000</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>81</v>
@@ -1784,17 +1796,17 @@
       <c r="I19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="3" t="s">
         <v>83</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0.1338613647683878</v>
-      </c>
-      <c r="L19" s="2" t="n">
-        <v>0.08623511202830189</v>
-      </c>
-      <c r="M19" s="3" t="n">
-        <v>-0.04762625274008594</v>
+        <v>0.3829540502131691</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>0.4499646605268794</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0.06701061031371025</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1805,19 +1817,19 @@
         <v>84</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>505878</v>
+        <v>806247</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>497703</v>
+        <v>585019</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.983839977227711</v>
+        <v>0.7256076611757936</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>4800000</v>
+        <v>6023000</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>5995000</v>
+        <v>6784000</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>85</v>
@@ -1829,13 +1841,13 @@
         <v>87</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>0.10539125</v>
+        <v>0.1338613647683878</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>0.08301968306922436</v>
-      </c>
-      <c r="M20" s="3" t="n">
-        <v>-0.02237156693077565</v>
+        <v>0.08623511202830189</v>
+      </c>
+      <c r="M20" s="4" t="n">
+        <v>-0.04762625274008594</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1846,19 +1858,19 @@
         <v>88</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>247484</v>
+        <v>505878</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>202725</v>
+        <v>497703</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.8191438638457436</v>
+        <v>0.983839977227711</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>1232000</v>
+        <v>4800000</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>1329000</v>
+        <v>5995000</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>89</v>
@@ -1870,13 +1882,13 @@
         <v>91</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.2008798701298701</v>
+        <v>0.10539125</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0.1525395033860045</v>
-      </c>
-      <c r="M21" s="3" t="n">
-        <v>-0.0483403667438656</v>
+        <v>0.08301968306922436</v>
+      </c>
+      <c r="M21" s="4" t="n">
+        <v>-0.02237156693077565</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1887,19 +1899,19 @@
         <v>92</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>872559</v>
+        <v>247484</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>880095</v>
+        <v>202725</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>1.00863666525702</v>
+        <v>0.8191438638457436</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>9311000</v>
+        <v>1232000</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>9918000</v>
+        <v>1329000</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>93</v>
@@ -1911,13 +1923,13 @@
         <v>95</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>0.09371270540221244</v>
+        <v>0.2008798701298701</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>0.08873714458560193</v>
-      </c>
-      <c r="M22" s="3" t="n">
-        <v>-0.004975560816610505</v>
+        <v>0.1525395033860045</v>
+      </c>
+      <c r="M22" s="4" t="n">
+        <v>-0.0483403667438656</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1928,19 +1940,19 @@
         <v>96</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>503176</v>
+        <v>872559</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>594379</v>
+        <v>880095</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.181254670334038</v>
+        <v>1.00863666525702</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>4390000</v>
+        <v>9311000</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>5482000</v>
+        <v>9918000</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>97</v>
@@ -1952,13 +1964,13 @@
         <v>99</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.1146186788154897</v>
+        <v>0.09371270540221244</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>0.1084237504560379</v>
-      </c>
-      <c r="M23" s="3" t="n">
-        <v>-0.006194928359451804</v>
+        <v>0.08873714458560193</v>
+      </c>
+      <c r="M23" s="4" t="n">
+        <v>-0.004975560816610505</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1969,19 +1981,19 @@
         <v>100</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>586751</v>
+        <v>503176</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>644903</v>
+        <v>594379</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>1.099108480428666</v>
+        <v>1.181254670334038</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>5129000</v>
+        <v>4390000</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>6076000</v>
+        <v>5482000</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>101</v>
@@ -1993,13 +2005,13 @@
         <v>103</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.1143987131994541</v>
+        <v>0.1146186788154897</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>0.106139400921659</v>
-      </c>
-      <c r="M24" s="3" t="n">
-        <v>-0.008259312277795111</v>
+        <v>0.1084237504560379</v>
+      </c>
+      <c r="M24" s="4" t="n">
+        <v>-0.006194928359451804</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2010,19 +2022,19 @@
         <v>104</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>374556</v>
+        <v>586751</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>445123</v>
+        <v>644903</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>1.188401734320102</v>
+        <v>1.099108480428666</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>2579000</v>
+        <v>5129000</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>2989000</v>
+        <v>6076000</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>105</v>
@@ -2034,13 +2046,13 @@
         <v>107</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>0.1452330360604886</v>
+        <v>0.1143987131994541</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>0.1489203747072599</v>
-      </c>
-      <c r="M25" s="2" t="n">
-        <v>0.003687338646771371</v>
+        <v>0.106139400921659</v>
+      </c>
+      <c r="M25" s="4" t="n">
+        <v>-0.008259312277795111</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2051,19 +2063,19 @@
         <v>108</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>142518</v>
+        <v>374556</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>171028</v>
+        <v>445123</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>1.200044906608288</v>
+        <v>1.188401734320102</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>800000</v>
+        <v>2579000</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>1032000</v>
+        <v>2989000</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>109</v>
@@ -2075,13 +2087,13 @@
         <v>111</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>0.1781475</v>
+        <v>0.1452330360604886</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>0.1657248062015504</v>
-      </c>
-      <c r="M26" s="3" t="n">
-        <v>-0.0124226937984496</v>
+        <v>0.1489203747072599</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>0.003687338646771371</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -2092,19 +2104,19 @@
         <v>112</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>715890</v>
+        <v>142518</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>826511</v>
+        <v>171028</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1.154522342818031</v>
+        <v>1.200044906608288</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>6664000</v>
+        <v>800000</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>10035000</v>
+        <v>1032000</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>113</v>
@@ -2116,13 +2128,13 @@
         <v>115</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.1074264705882353</v>
+        <v>0.1781475</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0.08236283009466866</v>
-      </c>
-      <c r="M27" s="3" t="n">
-        <v>-0.02506364049356663</v>
+        <v>0.1657248062015504</v>
+      </c>
+      <c r="M27" s="4" t="n">
+        <v>-0.0124226937984496</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -2133,19 +2145,19 @@
         <v>116</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>112126</v>
+        <v>715890</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>198167</v>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>1.76735993435956</v>
+        <v>826511</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>1.154522342818031</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>638000</v>
+        <v>6664000</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>757000</v>
+        <v>10035000</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>117</v>
@@ -2157,13 +2169,13 @@
         <v>119</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>0.1757460815047022</v>
+        <v>0.1074264705882353</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>0.261779392338177</v>
+        <v>0.08236283009466866</v>
       </c>
       <c r="M28" s="4" t="n">
-        <v>0.08603331083347485</v>
+        <v>-0.02506364049356663</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2174,19 +2186,19 @@
         <v>120</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>205221</v>
+        <v>112126</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>243161</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>1.184873867684106</v>
+        <v>198167</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>1.76735993435956</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>1221000</v>
+        <v>638000</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>2884000</v>
+        <v>757000</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>121</v>
@@ -2198,13 +2210,13 @@
         <v>123</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.1680761670761671</v>
+        <v>0.1757460815047022</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>0.08431380027739251</v>
+        <v>0.261779392338177</v>
       </c>
       <c r="M29" s="3" t="n">
-        <v>-0.08376236679877457</v>
+        <v>0.08603331083347485</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2215,19 +2227,19 @@
         <v>124</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>159071</v>
+        <v>205221</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>155987</v>
+        <v>243161</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.9806124309270703</v>
+        <v>1.184873867684106</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>1112000</v>
+        <v>1221000</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>1330000</v>
+        <v>2884000</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>125</v>
@@ -2239,13 +2251,13 @@
         <v>127</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>0.1430494604316547</v>
+        <v>0.1680761670761671</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>0.1172834586466165</v>
-      </c>
-      <c r="M30" s="3" t="n">
-        <v>-0.02576600178503813</v>
+        <v>0.08431380027739251</v>
+      </c>
+      <c r="M30" s="4" t="n">
+        <v>-0.08376236679877457</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2256,19 +2268,19 @@
         <v>128</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>1128254</v>
+        <v>159071</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>1014962</v>
+        <v>155987</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.8995864406419122</v>
+        <v>0.9806124309270703</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>7763000</v>
+        <v>1112000</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>8935000</v>
+        <v>1330000</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>129</v>
@@ -2280,13 +2292,13 @@
         <v>131</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>0.1453373695736185</v>
+        <v>0.1430494604316547</v>
       </c>
       <c r="L31" s="2" t="n">
-        <v>0.113593956351427</v>
-      </c>
-      <c r="M31" s="3" t="n">
-        <v>-0.03174341322219149</v>
+        <v>0.1172834586466165</v>
+      </c>
+      <c r="M31" s="4" t="n">
+        <v>-0.02576600178503813</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2297,19 +2309,19 @@
         <v>132</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>211433</v>
+        <v>1128254</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>246516</v>
+        <v>1014962</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>1.165929632554994</v>
+        <v>0.8995864406419122</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>1522000</v>
+        <v>7763000</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>2080000</v>
+        <v>8935000</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>133</v>
@@ -2321,13 +2333,13 @@
         <v>135</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>0.1389178712220762</v>
+        <v>0.1453373695736185</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>0.1185173076923077</v>
-      </c>
-      <c r="M32" s="3" t="n">
-        <v>-0.02040056352976853</v>
+        <v>0.113593956351427</v>
+      </c>
+      <c r="M32" s="4" t="n">
+        <v>-0.03174341322219149</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2338,19 +2350,19 @@
         <v>136</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>168955</v>
+        <v>211433</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>230353</v>
+        <v>246516</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>1.363398538072268</v>
+        <v>1.165929632554994</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>1582000</v>
+        <v>1522000</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>1894000</v>
+        <v>2080000</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>137</v>
@@ -2362,13 +2374,13 @@
         <v>139</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>0.1067983565107459</v>
+        <v>0.1389178712220762</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>0.1216224920802534</v>
-      </c>
-      <c r="M33" s="2" t="n">
-        <v>0.01482413556950754</v>
+        <v>0.1185173076923077</v>
+      </c>
+      <c r="M33" s="4" t="n">
+        <v>-0.02040056352976853</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2379,19 +2391,19 @@
         <v>140</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>1785650</v>
+        <v>168955</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>1345969</v>
+        <v>230353</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0.7537697757119256</v>
+        <v>1.363398538072268</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>18021000</v>
+        <v>1582000</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>19747000</v>
+        <v>1894000</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>141</v>
@@ -2403,13 +2415,13 @@
         <v>143</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>0.09908717607236002</v>
+        <v>0.1067983565107459</v>
       </c>
       <c r="L34" s="2" t="n">
-        <v>0.06816068263533702</v>
-      </c>
-      <c r="M34" s="3" t="n">
-        <v>-0.030926493437023</v>
+        <v>0.1216224920802534</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <v>0.01482413556950754</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2420,19 +2432,19 @@
         <v>144</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>1088486</v>
+        <v>1785650</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1169466</v>
+        <v>1345969</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>1.074396914613509</v>
+        <v>0.7537697757119256</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>10864000</v>
+        <v>18021000</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>11605000</v>
+        <v>19747000</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>145</v>
@@ -2444,13 +2456,13 @@
         <v>147</v>
       </c>
       <c r="K35" s="2" t="n">
-        <v>0.1001920103092784</v>
+        <v>0.09908717607236002</v>
       </c>
       <c r="L35" s="2" t="n">
-        <v>0.1007725980180957</v>
-      </c>
-      <c r="M35" s="2" t="n">
-        <v>0.0005805877088173039</v>
+        <v>0.06816068263533702</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <v>-0.030926493437023</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2461,19 +2473,19 @@
         <v>148</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>430751</v>
+        <v>1088486</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>549018</v>
+        <v>1169466</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>1.274560012629106</v>
+        <v>1.074396914613509</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>3149000</v>
+        <v>10864000</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>3907000</v>
+        <v>11605000</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>149</v>
@@ -2485,13 +2497,13 @@
         <v>151</v>
       </c>
       <c r="K36" s="2" t="n">
-        <v>0.1367897745315973</v>
+        <v>0.1001920103092784</v>
       </c>
       <c r="L36" s="2" t="n">
-        <v>0.1405216278474533</v>
+        <v>0.1007725980180957</v>
       </c>
       <c r="M36" s="2" t="n">
-        <v>0.00373185331585596</v>
+        <v>0.0005805877088173039</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2502,19 +2514,19 @@
         <v>152</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>346266</v>
+        <v>430751</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>339200</v>
+        <v>549018</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>0.9795937227449417</v>
+        <v>1.274560012629106</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>2860000</v>
+        <v>3149000</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>4025000</v>
+        <v>3907000</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>153</v>
@@ -2526,13 +2538,13 @@
         <v>155</v>
       </c>
       <c r="K37" s="2" t="n">
-        <v>0.121072027972028</v>
+        <v>0.1367897745315973</v>
       </c>
       <c r="L37" s="2" t="n">
-        <v>0.08427329192546584</v>
-      </c>
-      <c r="M37" s="3" t="n">
-        <v>-0.03679873604656213</v>
+        <v>0.1405216278474533</v>
+      </c>
+      <c r="M37" s="2" t="n">
+        <v>0.00373185331585596</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2543,19 +2555,19 @@
         <v>156</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>1311449</v>
+        <v>346266</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>1212824</v>
+        <v>339200</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0.9247969230980388</v>
+        <v>0.9795937227449417</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>11903000</v>
+        <v>2860000</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>12792000</v>
+        <v>4025000</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>157</v>
@@ -2567,13 +2579,13 @@
         <v>159</v>
       </c>
       <c r="K38" s="2" t="n">
-        <v>0.1101780223473074</v>
+        <v>0.121072027972028</v>
       </c>
       <c r="L38" s="2" t="n">
-        <v>0.09481113195747343</v>
-      </c>
-      <c r="M38" s="3" t="n">
-        <v>-0.01536689038983398</v>
+        <v>0.08427329192546584</v>
+      </c>
+      <c r="M38" s="4" t="n">
+        <v>-0.03679873604656213</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2584,19 +2596,19 @@
         <v>160</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>104531</v>
+        <v>1311449</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>90344</v>
+        <v>1212824</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>0.8642794960346691</v>
+        <v>0.9247969230980388</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>1006000</v>
+        <v>11903000</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>1056000</v>
+        <v>12792000</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>161</v>
@@ -2608,13 +2620,13 @@
         <v>163</v>
       </c>
       <c r="K39" s="2" t="n">
-        <v>0.1039075546719682</v>
+        <v>0.1101780223473074</v>
       </c>
       <c r="L39" s="2" t="n">
-        <v>0.0855530303030303</v>
-      </c>
-      <c r="M39" s="3" t="n">
-        <v>-0.01835452436893789</v>
+        <v>0.09481113195747343</v>
+      </c>
+      <c r="M39" s="4" t="n">
+        <v>-0.01536689038983398</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2625,19 +2637,19 @@
         <v>164</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>387716</v>
+        <v>104531</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>531594</v>
+        <v>90344</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>1.371091211092655</v>
+        <v>0.8642794960346691</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>3501000</v>
+        <v>1006000</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>4895000</v>
+        <v>1056000</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>165</v>
@@ -2649,13 +2661,13 @@
         <v>167</v>
       </c>
       <c r="K40" s="2" t="n">
-        <v>0.1107443587546415</v>
+        <v>0.1039075546719682</v>
       </c>
       <c r="L40" s="2" t="n">
-        <v>0.1085993871297242</v>
-      </c>
-      <c r="M40" s="3" t="n">
-        <v>-0.002144971624917322</v>
+        <v>0.0855530303030303</v>
+      </c>
+      <c r="M40" s="4" t="n">
+        <v>-0.01835452436893789</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2666,19 +2678,19 @@
         <v>168</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>108574</v>
+        <v>387716</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>119014</v>
+        <v>531594</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>1.096155617366957</v>
+        <v>1.371091211092655</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>697000</v>
+        <v>3501000</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>858000</v>
+        <v>4895000</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>169</v>
@@ -2690,13 +2702,13 @@
         <v>171</v>
       </c>
       <c r="K41" s="2" t="n">
-        <v>0.1557733142037303</v>
+        <v>0.1107443587546415</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>0.1387109557109557</v>
-      </c>
-      <c r="M41" s="3" t="n">
-        <v>-0.01706235849277457</v>
+        <v>0.1085993871297242</v>
+      </c>
+      <c r="M41" s="4" t="n">
+        <v>-0.002144971624917322</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2707,19 +2719,19 @@
         <v>172</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>553286</v>
+        <v>108574</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>710595</v>
+        <v>119014</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>1.284317694646169</v>
+        <v>1.096155617366957</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>4894000</v>
+        <v>697000</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>6595000</v>
+        <v>858000</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>173</v>
@@ -2731,13 +2743,13 @@
         <v>175</v>
       </c>
       <c r="K42" s="2" t="n">
-        <v>0.1130539436044136</v>
+        <v>0.1557733142037303</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>0.1077475360121304</v>
-      </c>
-      <c r="M42" s="3" t="n">
-        <v>-0.005306407592283166</v>
+        <v>0.1387109557109557</v>
+      </c>
+      <c r="M42" s="4" t="n">
+        <v>-0.01706235849277457</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2748,19 +2760,19 @@
         <v>176</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>4791526</v>
+        <v>553286</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>6291763</v>
+        <v>710595</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>1.313102130719942</v>
+        <v>1.284317694646169</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>17057000</v>
+        <v>4894000</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>27430000</v>
+        <v>6595000</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>177</v>
@@ -2772,36 +2784,36 @@
         <v>179</v>
       </c>
       <c r="K43" s="2" t="n">
-        <v>0.280912587207598</v>
+        <v>0.1130539436044136</v>
       </c>
       <c r="L43" s="2" t="n">
-        <v>0.2293752460809333</v>
-      </c>
-      <c r="M43" s="3" t="n">
-        <v>-0.05153734112666475</v>
+        <v>0.1077475360121304</v>
+      </c>
+      <c r="M43" s="4" t="n">
+        <v>-0.005306407592283166</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>193286</v>
+        <v>4791526</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>285501</v>
+        <v>6291763</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>1.477090942954999</v>
+        <v>1.313102130719942</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>1731000</v>
+        <v>17057000</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>2991000</v>
+        <v>27430000</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>181</v>
@@ -2813,13 +2825,13 @@
         <v>183</v>
       </c>
       <c r="K44" s="2" t="n">
-        <v>0.1116614673599076</v>
+        <v>0.280912587207598</v>
       </c>
       <c r="L44" s="2" t="n">
-        <v>0.09545336008024072</v>
-      </c>
-      <c r="M44" s="3" t="n">
-        <v>-0.01620810727966684</v>
+        <v>0.2293752460809333</v>
+      </c>
+      <c r="M44" s="4" t="n">
+        <v>-0.05153734112666475</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2830,19 +2842,19 @@
         <v>184</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>752648</v>
+        <v>193286</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>804032</v>
+        <v>285501</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>1.068270958004273</v>
+        <v>1.477090942954999</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>6217000</v>
+        <v>1731000</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>8368000</v>
+        <v>2991000</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>185</v>
@@ -2854,13 +2866,13 @@
         <v>187</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>0.1210628920701303</v>
+        <v>0.1116614673599076</v>
       </c>
       <c r="L45" s="2" t="n">
-        <v>0.09608413001912046</v>
-      </c>
-      <c r="M45" s="3" t="n">
-        <v>-0.02497876205100982</v>
+        <v>0.09545336008024072</v>
+      </c>
+      <c r="M45" s="4" t="n">
+        <v>-0.01620810727966684</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2871,19 +2883,19 @@
         <v>188</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>72022</v>
+        <v>752648</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>84362</v>
+        <v>804032</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>1.171336536058427</v>
+        <v>1.068270958004273</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>565000</v>
+        <v>6217000</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>626000</v>
+        <v>8368000</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>189</v>
@@ -2895,13 +2907,13 @@
         <v>191</v>
       </c>
       <c r="K46" s="2" t="n">
-        <v>0.1274725663716814</v>
+        <v>0.1210628920701303</v>
       </c>
       <c r="L46" s="2" t="n">
-        <v>0.1347635782747604</v>
-      </c>
-      <c r="M46" s="2" t="n">
-        <v>0.007291011903078959</v>
+        <v>0.09608413001912046</v>
+      </c>
+      <c r="M46" s="4" t="n">
+        <v>-0.02497876205100982</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2912,19 +2924,19 @@
         <v>192</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>763310</v>
+        <v>72022</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>769134</v>
+        <v>84362</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>1.007629927552371</v>
+        <v>1.171336536058427</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>4903000</v>
+        <v>565000</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>7160000</v>
+        <v>626000</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>193</v>
@@ -2936,13 +2948,13 @@
         <v>195</v>
       </c>
       <c r="K47" s="2" t="n">
-        <v>0.1556822353661024</v>
+        <v>0.1274725663716814</v>
       </c>
       <c r="L47" s="2" t="n">
-        <v>0.1074209497206704</v>
-      </c>
-      <c r="M47" s="3" t="n">
-        <v>-0.04826128564543199</v>
+        <v>0.1347635782747604</v>
+      </c>
+      <c r="M47" s="2" t="n">
+        <v>0.007291011903078959</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2953,19 +2965,19 @@
         <v>196</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>478723</v>
+        <v>763310</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>552182</v>
+        <v>769134</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>1.153447818467047</v>
+        <v>1.007629927552371</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>4905000</v>
+        <v>4903000</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>5768000</v>
+        <v>7160000</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>197</v>
@@ -2977,13 +2989,13 @@
         <v>199</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>0.09759898063200816</v>
+        <v>0.1556822353661024</v>
       </c>
       <c r="L48" s="2" t="n">
-        <v>0.09573196948682386</v>
-      </c>
-      <c r="M48" s="3" t="n">
-        <v>-0.001867011145184297</v>
+        <v>0.1074209497206704</v>
+      </c>
+      <c r="M48" s="4" t="n">
+        <v>-0.04826128564543199</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2994,19 +3006,19 @@
         <v>200</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>207783</v>
+        <v>478723</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>195015</v>
+        <v>552182</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0.9385512770534644</v>
+        <v>1.153447818467047</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>1793000</v>
+        <v>4905000</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>1841000</v>
+        <v>5768000</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>201</v>
@@ -3018,36 +3030,36 @@
         <v>203</v>
       </c>
       <c r="K49" s="2" t="n">
-        <v>0.1158856664807585</v>
+        <v>0.09759898063200816</v>
       </c>
       <c r="L49" s="2" t="n">
-        <v>0.1059288430200978</v>
-      </c>
-      <c r="M49" s="3" t="n">
-        <v>-0.009956823460660721</v>
+        <v>0.09573196948682386</v>
+      </c>
+      <c r="M49" s="4" t="n">
+        <v>-0.001867011145184297</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>122904</v>
+        <v>207783</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>163161</v>
+        <v>195015</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>1.327548330404218</v>
+        <v>0.9385512770534644</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>454000</v>
+        <v>1793000</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>587000</v>
+        <v>1841000</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>205</v>
@@ -3059,36 +3071,36 @@
         <v>207</v>
       </c>
       <c r="K50" s="2" t="n">
-        <v>0.2707136563876652</v>
+        <v>0.1158856664807585</v>
       </c>
       <c r="L50" s="2" t="n">
-        <v>0.2779574105621806</v>
-      </c>
-      <c r="M50" s="2" t="n">
-        <v>0.007243754174515393</v>
+        <v>0.1059288430200978</v>
+      </c>
+      <c r="M50" s="4" t="n">
+        <v>-0.009956823460660721</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="4" t="n">
-        <v>33551626</v>
-      </c>
-      <c r="D51" s="4" t="n">
-        <v>36871338</v>
+      <c r="C51" s="2" t="n">
+        <v>122904</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>163161</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>1.098943401431573</v>
-      </c>
-      <c r="F51" s="4" t="n">
-        <v>249623000</v>
-      </c>
-      <c r="G51" s="4" t="n">
-        <v>320897000</v>
+        <v>1.327548330404218</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>454000</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>587000</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>209</v>
@@ -3100,12 +3112,53 @@
         <v>211</v>
       </c>
       <c r="K51" s="2" t="n">
+        <v>0.2707136563876652</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0.2779574105621806</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>0.007243754174515393</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>33551626</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>36871338</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>1.098943401431573</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>249623000</v>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>320897000</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K52" s="2" t="n">
         <v>0.1344091930631392</v>
       </c>
-      <c r="L51" s="2" t="n">
+      <c r="L52" s="2" t="n">
         <v>0.1149008498053893</v>
       </c>
-      <c r="M51" s="3" t="n">
+      <c r="M52" s="4" t="n">
         <v>-0.01950834325774996</v>
       </c>
     </row>

</xml_diff>